<commit_message>
worked on micro BOM
</commit_message>
<xml_diff>
--- a/micro/Design/RTC Resistor Supply Calulations.xlsx
+++ b/micro/Design/RTC Resistor Supply Calulations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User070\scat0009\Documents\Repositories\BoSL-nano\micro\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7207FE5A-92EC-46B7-8C2C-CAF7DB133BCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5278B764-721F-4AE5-99FA-01263FADE1C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{250E95CC-4025-44BB-A6D6-27FA839C01FC}"/>
   </bookViews>
@@ -3308,15 +3308,15 @@
       </c>
       <c r="B4" s="1">
         <f ca="1">C4</f>
-        <v>2918418.5014288216</v>
+        <v>2819620.4414420296</v>
       </c>
       <c r="C4" s="1">
         <f ca="1">B7/D4</f>
-        <v>3700628.953791779</v>
+        <v>3816109.5847871359</v>
       </c>
       <c r="D4" s="1">
         <f ca="1">(0.97+0.505*(B7-3.1)+0.224*(B7-3.1)^2+0.04*(B7-3.1)^3+0.0063*(B7-3.1)^4)/1000000</f>
-        <v>9.4915231516207899E-7</v>
+        <v>9.6718984084893922E-7</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -3325,7 +3325,7 @@
       </c>
       <c r="B6" s="1">
         <f ca="1">B1/(B2+(1/B3+1/B4)^-1)</f>
-        <v>1.5383554915458748E-6</v>
+        <v>1.5474242848027348E-6</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B7" s="1">
         <f ca="1">B1*(1/B3+1/B4)^-1/(B2+(1/B3+1/B4)^-1)</f>
-        <v>2.7697291897343876</v>
+        <v>2.7271058614271455</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="B8" s="1">
         <f ca="1">B7/B4</f>
-        <v>9.4905140862366471E-7</v>
+        <v>9.6718899513738475E-7</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>

</xml_diff>